<commit_message>
0915/Working with Excel files part2
</commit_message>
<xml_diff>
--- a/DataTables and Excel Automation with Studio/Data/Results.xlsx
+++ b/DataTables and Excel Automation with Studio/Data/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip-ioan.zirbo\Documents\UiPath\FilteringEmployeeData\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1020a\OneDrive\바탕 화면\clone\DataTables and Excel Automation with Studio\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09F5EBD-72FF-4595-B0FD-9241C31D2DB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853C82CE-82A2-48B5-866F-596C0C99359E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="-11955" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,60 +25,309 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Age</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Income</t>
-  </si>
-  <si>
-    <t>Beiriger,  Terry J</t>
-  </si>
-  <si>
-    <t>Bloome Jr,  Robert A</t>
-  </si>
-  <si>
-    <t>Caraballo,  Alexander</t>
-  </si>
-  <si>
-    <t>Deenihan,  Brendan D</t>
-  </si>
-  <si>
-    <t>Edeling,  Timothy S</t>
-  </si>
-  <si>
-    <t>Lopez,  Baudilio</t>
-  </si>
-  <si>
-    <t>Mc Gee Jr,  John T</t>
-  </si>
-  <si>
-    <t>Pope,  Terrence L</t>
-  </si>
-  <si>
-    <t>Stachula,  Christophe D</t>
-  </si>
-  <si>
-    <t>Tully,  Sean F</t>
-  </si>
-  <si>
-    <t>Yonover,  Scott D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alfich,  Fred T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Almaguer,  Philip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anderson,  Elizer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Arcos,  Xavier</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brown,  Michael D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cacciatore,  Jon J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clark,  Richard B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Collier Jr,  Kent E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consago,  Daniel F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dallio,  Matthew J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Davis,  Crystal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>English,  Cheryl D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fineron,  Raymond J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foster,  Shanita L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frank,  Robert</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Garcia,  Louis J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gauthier,  Klanci J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gorske,  Judith A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gutrich,  Patrick K</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hariri,  Mazyar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insalaco,  John A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jablonsky,  Daniel T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Johnson,  Bernard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Johnson-Smalley,  Christine L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jones,  Richard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Josephs,  Patrick R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kaczynski,  Michael J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kichura,  Christopher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lacivita,  Mark A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lewis,  Byron</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lichay,  Kenneth A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lopez,  Rochelle A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lowery,  Joseph L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mcbride,  Thomas J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mionskowski,  Erika J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Negrillo,  M Gloria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Newell,  Lolita M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Noys,  Craig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Olortegui,  Darwin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ontiveros,  Robert A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ortiz,  Edith M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perez,  Robert M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pina,  Richard C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ptak,  Carolyn M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reynolds,  Kimberly R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Romero,  Miguel A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schnoor,  Roy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Segreti,  Patricia J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Soderlund,  Christopher J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sorrell,  Esther L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spears Jr,  Willie L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starks,  Alvin D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sumner,  Brian N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thomas,  Trina M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toledo,  Ramon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Torres,  Hector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vander Vaart,  Martin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vasquez,  Vincent A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Velazquez,  Martin J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitek,  Kathleen A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Walter,  Karen A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Warfield,  Melvin E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Watanabe,  Scott A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wells,  Pennline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Williams,  Demond</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Williams,  Linda F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wyatt,  Todd H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zagloba,  Amanda L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -106,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -384,19 +633,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.296875" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -415,76 +664,76 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>117078</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>97968</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3">
-        <v>105918</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4">
-        <v>116724</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19656</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>116724</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>61356</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>110370</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>106920</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>94236</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>106920</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>67212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -492,43 +741,672 @@
         <v>27</v>
       </c>
       <c r="C9">
-        <v>103590</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>89718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C10">
-        <v>106920</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>93745.600000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11">
-        <v>103590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>80778</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>44568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>66684</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>90798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>99252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>26</v>
+      </c>
+      <c r="C18">
+        <v>25152.400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>91068</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>85680</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>89718</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>97968</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>25</v>
+      </c>
+      <c r="C24">
+        <v>42099.199999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+      <c r="C25">
+        <v>43920</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>127824</v>
+      <c r="B26">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>40560</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>89718</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>46206</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>80778</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>88968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>28</v>
+      </c>
+      <c r="C32">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>71780.800000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>85680</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>23</v>
+      </c>
+      <c r="C37">
+        <v>50496</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39">
+        <v>29</v>
+      </c>
+      <c r="C39">
+        <v>72862.399999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40">
+        <v>27</v>
+      </c>
+      <c r="C40">
+        <v>77280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>28</v>
+      </c>
+      <c r="C42">
+        <v>92316</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>25</v>
+      </c>
+      <c r="C43">
+        <v>89718</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>28</v>
+      </c>
+      <c r="C44">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45">
+        <v>80424</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>27</v>
+      </c>
+      <c r="C46">
+        <v>69888</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>29</v>
+      </c>
+      <c r="C48">
+        <v>59796</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49">
+        <v>24</v>
+      </c>
+      <c r="C49">
+        <v>55428</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>80778</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <v>83100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52">
+        <v>24</v>
+      </c>
+      <c r="C52">
+        <v>86520</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53">
+        <v>29</v>
+      </c>
+      <c r="C53">
+        <v>97020</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>98675.199999999997</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55">
+        <v>28</v>
+      </c>
+      <c r="C55">
+        <v>89718</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>79040</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <v>16151.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58">
+        <v>24</v>
+      </c>
+      <c r="C58">
+        <v>72862.399999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59">
+        <v>25</v>
+      </c>
+      <c r="C59">
+        <v>80778</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>22</v>
+      </c>
+      <c r="C61">
+        <v>93024</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62">
+        <v>27</v>
+      </c>
+      <c r="C62">
+        <v>83616</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63">
+        <v>29</v>
+      </c>
+      <c r="C63">
+        <v>80916</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>26</v>
+      </c>
+      <c r="C64">
+        <v>72840</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>29</v>
+      </c>
+      <c r="C65">
+        <v>19656</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>17945.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>41952</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68">
+        <v>23</v>
+      </c>
+      <c r="C68">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69">
+        <v>23</v>
+      </c>
+      <c r="C69">
+        <v>53796</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>